<commit_message>
Perf - highlight relevant analyzers in system-io-aggregated
</commit_message>
<xml_diff>
--- a/docs/ReportAnalyzer-analyzers-versions/2017-04-21-systamio/aggregated.xlsx
+++ b/docs/ReportAnalyzer-analyzers-versions/2017-04-21-systamio/aggregated.xlsx
@@ -211,7 +211,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,6 +391,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -552,9 +558,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - zvýraznenie1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -913,7 +921,7 @@
   <dimension ref="A1:CX9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,10 +931,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="3">
         <f>TRIMMEAN(C1:CX1,0.3)</f>
         <v>18.677542857142857</v>
       </c>
@@ -1850,10 +1858,10 @@
       </c>
     </row>
     <row r="4" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <f t="shared" si="0"/>
         <v>7.8746142857142871</v>
       </c>
@@ -2159,10 +2167,10 @@
       </c>
     </row>
     <row r="5" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="3">
         <f t="shared" si="0"/>
         <v>7.6136571428571411</v>
       </c>
@@ -3086,10 +3094,10 @@
       </c>
     </row>
     <row r="8" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="3">
         <f t="shared" si="0"/>
         <v>1.2922571428571432</v>
       </c>
@@ -3395,10 +3403,10 @@
       </c>
     </row>
     <row r="9" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="3">
         <f t="shared" si="0"/>
         <v>0.53207142857142864</v>
       </c>

</xml_diff>

<commit_message>
Perf - clean up docs forlder
</commit_message>
<xml_diff>
--- a/docs/ReportAnalyzer-analyzers-versions/2017-04-21-systamio/aggregated.xlsx
+++ b/docs/ReportAnalyzer-analyzers-versions/2017-04-21-systamio/aggregated.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12525" windowHeight="2055"/>
   </bookViews>
   <sheets>
     <sheet name="aggregated" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -397,6 +397,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -558,11 +564,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - zvýraznenie1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -920,631 +928,631 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CX9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="115.28515625" customWidth="1"/>
+    <col min="1" max="1" width="113.7109375" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:102" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3">
-        <f>TRIMMEAN(C1:CX1,0.3)</f>
-        <v>18.677542857142857</v>
-      </c>
-      <c r="C1">
+      <c r="B1" s="5">
+        <f t="shared" ref="B1:B8" si="0">TRIMMEAN(C1:CX1,0.25)</f>
+        <v>18.677302631578947</v>
+      </c>
+      <c r="C1" s="4">
         <v>17.544</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="4">
         <v>16.588999999999999</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="4">
         <v>19.074000000000002</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="4">
         <v>17.344000000000001</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="4">
         <v>17.344000000000001</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="4">
         <v>19.613</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="4">
         <v>17.036000000000001</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="4">
         <v>17.690999999999999</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="4">
         <v>18.082000000000001</v>
       </c>
-      <c r="L1">
+      <c r="L1" s="4">
         <v>19.175999999999998</v>
       </c>
-      <c r="M1">
+      <c r="M1" s="4">
         <v>18.564</v>
       </c>
-      <c r="N1">
+      <c r="N1" s="4">
         <v>18.408000000000001</v>
       </c>
-      <c r="O1">
+      <c r="O1" s="4">
         <v>18.68</v>
       </c>
-      <c r="P1">
+      <c r="P1" s="4">
         <v>20.388000000000002</v>
       </c>
-      <c r="Q1">
+      <c r="Q1" s="4">
         <v>18.803999999999998</v>
       </c>
-      <c r="R1">
+      <c r="R1" s="4">
         <v>19.309000000000001</v>
       </c>
-      <c r="S1">
+      <c r="S1" s="4">
         <v>18.527999999999999</v>
       </c>
-      <c r="T1">
+      <c r="T1" s="4">
         <v>18.872</v>
       </c>
-      <c r="U1">
+      <c r="U1" s="4">
         <v>17.89</v>
       </c>
-      <c r="V1">
+      <c r="V1" s="4">
         <v>17.59</v>
       </c>
-      <c r="W1">
+      <c r="W1" s="4">
         <v>18.664000000000001</v>
       </c>
-      <c r="X1">
+      <c r="X1" s="4">
         <v>19.373999999999999</v>
       </c>
-      <c r="Y1">
+      <c r="Y1" s="4">
         <v>18.707999999999998</v>
       </c>
-      <c r="Z1">
+      <c r="Z1" s="4">
         <v>17.459</v>
       </c>
-      <c r="AA1">
+      <c r="AA1" s="4">
         <v>17.803999999999998</v>
       </c>
-      <c r="AB1">
+      <c r="AB1" s="4">
         <v>17.677</v>
       </c>
-      <c r="AC1">
+      <c r="AC1" s="4">
         <v>18.739999999999998</v>
       </c>
-      <c r="AD1">
+      <c r="AD1" s="4">
         <v>18.986999999999998</v>
       </c>
-      <c r="AE1">
+      <c r="AE1" s="4">
         <v>18.242000000000001</v>
       </c>
-      <c r="AF1">
+      <c r="AF1" s="4">
         <v>19.564</v>
       </c>
-      <c r="AG1">
+      <c r="AG1" s="4">
         <v>18.87</v>
       </c>
-      <c r="AH1">
+      <c r="AH1" s="4">
         <v>20.196000000000002</v>
       </c>
-      <c r="AI1">
+      <c r="AI1" s="4">
         <v>20.678999999999998</v>
       </c>
-      <c r="AJ1">
+      <c r="AJ1" s="4">
         <v>17.565999999999999</v>
       </c>
-      <c r="AK1">
+      <c r="AK1" s="4">
         <v>18.518000000000001</v>
       </c>
-      <c r="AL1">
+      <c r="AL1" s="4">
         <v>18.027999999999999</v>
       </c>
-      <c r="AM1">
+      <c r="AM1" s="4">
         <v>20.768999999999998</v>
       </c>
-      <c r="AN1">
+      <c r="AN1" s="4">
         <v>17.443000000000001</v>
       </c>
-      <c r="AO1">
+      <c r="AO1" s="4">
         <v>19.082999999999998</v>
       </c>
-      <c r="AP1">
+      <c r="AP1" s="4">
         <v>19.202999999999999</v>
       </c>
-      <c r="AQ1">
+      <c r="AQ1" s="4">
         <v>20.273</v>
       </c>
-      <c r="AR1">
+      <c r="AR1" s="4">
         <v>19.864999999999998</v>
       </c>
-      <c r="AS1">
+      <c r="AS1" s="4">
         <v>19.643999999999998</v>
       </c>
-      <c r="AT1">
+      <c r="AT1" s="4">
         <v>18.931999999999999</v>
       </c>
-      <c r="AU1">
+      <c r="AU1" s="4">
         <v>19.420999999999999</v>
       </c>
-      <c r="AV1">
+      <c r="AV1" s="4">
         <v>19.773</v>
       </c>
-      <c r="AW1">
+      <c r="AW1" s="4">
         <v>17.692</v>
       </c>
-      <c r="AX1">
+      <c r="AX1" s="4">
         <v>19.192</v>
       </c>
-      <c r="AY1">
+      <c r="AY1" s="4">
         <v>17.617999999999999</v>
       </c>
-      <c r="AZ1">
+      <c r="AZ1" s="4">
         <v>18.521999999999998</v>
       </c>
-      <c r="BA1">
+      <c r="BA1" s="4">
         <v>19.625</v>
       </c>
-      <c r="BB1">
+      <c r="BB1" s="4">
         <v>20.379000000000001</v>
       </c>
-      <c r="BC1">
+      <c r="BC1" s="4">
         <v>18.344000000000001</v>
       </c>
-      <c r="BD1">
+      <c r="BD1" s="4">
         <v>18.774999999999999</v>
       </c>
-      <c r="BE1">
+      <c r="BE1" s="4">
         <v>18.443999999999999</v>
       </c>
-      <c r="BF1">
+      <c r="BF1" s="4">
         <v>18.189</v>
       </c>
-      <c r="BG1">
+      <c r="BG1" s="4">
         <v>19.292999999999999</v>
       </c>
-      <c r="BH1">
+      <c r="BH1" s="4">
         <v>18.693999999999999</v>
       </c>
-      <c r="BI1">
+      <c r="BI1" s="4">
         <v>16.683</v>
       </c>
-      <c r="BJ1">
+      <c r="BJ1" s="4">
         <v>17.803999999999998</v>
       </c>
-      <c r="BK1">
+      <c r="BK1" s="4">
         <v>18.149999999999999</v>
       </c>
-      <c r="BL1">
+      <c r="BL1" s="4">
         <v>17.655999999999999</v>
       </c>
-      <c r="BM1">
+      <c r="BM1" s="4">
         <v>18.696000000000002</v>
       </c>
-      <c r="BN1">
+      <c r="BN1" s="4">
         <v>18.021999999999998</v>
       </c>
-      <c r="BO1">
+      <c r="BO1" s="4">
         <v>17.765000000000001</v>
       </c>
-      <c r="BP1">
+      <c r="BP1" s="4">
         <v>20.225999999999999</v>
       </c>
-      <c r="BQ1">
+      <c r="BQ1" s="4">
         <v>17.597999999999999</v>
       </c>
-      <c r="BR1">
+      <c r="BR1" s="4">
         <v>18.123999999999999</v>
       </c>
-      <c r="BS1">
+      <c r="BS1" s="4">
         <v>18.809999999999999</v>
       </c>
-      <c r="BT1">
+      <c r="BT1" s="4">
         <v>20.317</v>
       </c>
-      <c r="BU1">
+      <c r="BU1" s="4">
         <v>19.983000000000001</v>
       </c>
-      <c r="BV1">
+      <c r="BV1" s="4">
         <v>17.507000000000001</v>
       </c>
-      <c r="BW1">
+      <c r="BW1" s="4">
         <v>19.207000000000001</v>
       </c>
-      <c r="BX1">
+      <c r="BX1" s="4">
         <v>18.11</v>
       </c>
-      <c r="BY1">
+      <c r="BY1" s="4">
         <v>17.661000000000001</v>
       </c>
-      <c r="BZ1">
+      <c r="BZ1" s="4">
         <v>19.515000000000001</v>
       </c>
-      <c r="CA1">
+      <c r="CA1" s="4">
         <v>18.959</v>
       </c>
-      <c r="CB1">
+      <c r="CB1" s="4">
         <v>19.169</v>
       </c>
-      <c r="CC1">
+      <c r="CC1" s="4">
         <v>18.556999999999999</v>
       </c>
-      <c r="CD1">
+      <c r="CD1" s="4">
         <v>18.905000000000001</v>
       </c>
-      <c r="CE1">
+      <c r="CE1" s="4">
         <v>17.917000000000002</v>
       </c>
-      <c r="CF1">
+      <c r="CF1" s="4">
         <v>19.536999999999999</v>
       </c>
-      <c r="CG1">
+      <c r="CG1" s="4">
         <v>19.853000000000002</v>
       </c>
-      <c r="CH1">
+      <c r="CH1" s="4">
         <v>18.591000000000001</v>
       </c>
-      <c r="CI1">
+      <c r="CI1" s="4">
         <v>19.742000000000001</v>
       </c>
-      <c r="CJ1">
+      <c r="CJ1" s="4">
         <v>17.789000000000001</v>
       </c>
-      <c r="CK1">
+      <c r="CK1" s="4">
         <v>19.053999999999998</v>
       </c>
-      <c r="CL1">
+      <c r="CL1" s="4">
         <v>18.030999999999999</v>
       </c>
-      <c r="CM1">
+      <c r="CM1" s="4">
         <v>17.901</v>
       </c>
-      <c r="CN1">
+      <c r="CN1" s="4">
         <v>19.079999999999998</v>
       </c>
-      <c r="CO1">
+      <c r="CO1" s="4">
         <v>19.943999999999999</v>
       </c>
-      <c r="CP1">
+      <c r="CP1" s="4">
         <v>19.454000000000001</v>
       </c>
-      <c r="CQ1">
+      <c r="CQ1" s="4">
         <v>19.449000000000002</v>
       </c>
-      <c r="CR1">
+      <c r="CR1" s="4">
         <v>18.654</v>
       </c>
-      <c r="CS1">
+      <c r="CS1" s="4">
         <v>19.66</v>
       </c>
-      <c r="CT1">
+      <c r="CT1" s="4">
         <v>18.609000000000002</v>
       </c>
-      <c r="CU1">
+      <c r="CU1" s="4">
         <v>17.481999999999999</v>
       </c>
-      <c r="CV1">
+      <c r="CV1" s="4">
         <v>19.074000000000002</v>
       </c>
-      <c r="CW1">
+      <c r="CW1" s="4">
         <v>19.545999999999999</v>
       </c>
-      <c r="CX1">
+      <c r="CX1" s="4">
         <v>18.367999999999999</v>
       </c>
     </row>
-    <row r="2" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:102" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <f t="shared" ref="B2:B9" si="0">TRIMMEAN(C2:CX2,0.3)</f>
-        <v>10.924828571428568</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="5">
+        <f t="shared" si="0"/>
+        <v>10.926947368421049</v>
+      </c>
+      <c r="C2" s="4">
         <v>10.371</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>10.845000000000001</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>11.015000000000001</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="4">
         <v>9.8460000000000001</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="4">
         <v>9.8460000000000001</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="4">
         <v>11.743</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="4">
         <v>10.239000000000001</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="4">
         <v>11.590999999999999</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="4">
         <v>12.148999999999999</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="4">
         <v>10.635999999999999</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="4">
         <v>10.585000000000001</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="4">
         <v>11.099</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="4">
         <v>10.472</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="4">
         <v>12.563000000000001</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="4">
         <v>11.840999999999999</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="4">
         <v>11.31</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="4">
         <v>9.6479999999999997</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="4">
         <v>11.042</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="4">
         <v>10.486000000000001</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="4">
         <v>10.138</v>
       </c>
-      <c r="W2">
+      <c r="W2" s="4">
         <v>10.464</v>
       </c>
-      <c r="X2">
+      <c r="X2" s="4">
         <v>11.715</v>
       </c>
-      <c r="Y2">
+      <c r="Y2" s="4">
         <v>10.621</v>
       </c>
-      <c r="Z2">
+      <c r="Z2" s="4">
         <v>10.685</v>
       </c>
-      <c r="AA2">
+      <c r="AA2" s="4">
         <v>9.5589999999999993</v>
       </c>
-      <c r="AB2">
+      <c r="AB2" s="4">
         <v>10.052</v>
       </c>
-      <c r="AC2">
+      <c r="AC2" s="4">
         <v>11.565</v>
       </c>
-      <c r="AD2">
+      <c r="AD2" s="4">
         <v>10.397</v>
       </c>
-      <c r="AE2">
+      <c r="AE2" s="4">
         <v>11.737</v>
       </c>
-      <c r="AF2">
+      <c r="AF2" s="4">
         <v>11.778</v>
       </c>
-      <c r="AG2">
+      <c r="AG2" s="4">
         <v>10.906000000000001</v>
       </c>
-      <c r="AH2">
+      <c r="AH2" s="4">
         <v>9.7449999999999992</v>
       </c>
-      <c r="AI2">
+      <c r="AI2" s="4">
         <v>10.098000000000001</v>
       </c>
-      <c r="AJ2">
+      <c r="AJ2" s="4">
         <v>11.778</v>
       </c>
-      <c r="AK2">
+      <c r="AK2" s="4">
         <v>10.927</v>
       </c>
-      <c r="AL2">
+      <c r="AL2" s="4">
         <v>12.253</v>
       </c>
-      <c r="AM2">
+      <c r="AM2" s="4">
         <v>11.244999999999999</v>
       </c>
-      <c r="AN2">
+      <c r="AN2" s="4">
         <v>10.602</v>
       </c>
-      <c r="AO2">
+      <c r="AO2" s="4">
         <v>10.071999999999999</v>
       </c>
-      <c r="AP2">
+      <c r="AP2" s="4">
         <v>12.243</v>
       </c>
-      <c r="AQ2">
+      <c r="AQ2" s="4">
         <v>10.680999999999999</v>
       </c>
-      <c r="AR2">
+      <c r="AR2" s="4">
         <v>11.067</v>
       </c>
-      <c r="AS2">
+      <c r="AS2" s="4">
         <v>11.965</v>
       </c>
-      <c r="AT2">
+      <c r="AT2" s="4">
         <v>11.894</v>
       </c>
-      <c r="AU2">
+      <c r="AU2" s="4">
         <v>11.247</v>
       </c>
-      <c r="AV2">
+      <c r="AV2" s="4">
         <v>10.958</v>
       </c>
-      <c r="AW2">
+      <c r="AW2" s="4">
         <v>11.316000000000001</v>
       </c>
-      <c r="AX2">
+      <c r="AX2" s="4">
         <v>10.727</v>
       </c>
-      <c r="AY2">
+      <c r="AY2" s="4">
         <v>10.71</v>
       </c>
-      <c r="AZ2">
+      <c r="AZ2" s="4">
         <v>11.805999999999999</v>
       </c>
-      <c r="BA2">
+      <c r="BA2" s="4">
         <v>10.545</v>
       </c>
-      <c r="BB2">
+      <c r="BB2" s="4">
         <v>11.407</v>
       </c>
-      <c r="BC2">
+      <c r="BC2" s="4">
         <v>11.67</v>
       </c>
-      <c r="BD2">
+      <c r="BD2" s="4">
         <v>10.87</v>
       </c>
-      <c r="BE2">
+      <c r="BE2" s="4">
         <v>12.151</v>
       </c>
-      <c r="BF2">
+      <c r="BF2" s="4">
         <v>11.102</v>
       </c>
-      <c r="BG2">
+      <c r="BG2" s="4">
         <v>10.391</v>
       </c>
-      <c r="BH2">
+      <c r="BH2" s="4">
         <v>10.324</v>
       </c>
-      <c r="BI2">
+      <c r="BI2" s="4">
         <v>10.89</v>
       </c>
-      <c r="BJ2">
+      <c r="BJ2" s="4">
         <v>12.163</v>
       </c>
-      <c r="BK2">
+      <c r="BK2" s="4">
         <v>9.9529999999999994</v>
       </c>
-      <c r="BL2">
+      <c r="BL2" s="4">
         <v>10.69</v>
       </c>
-      <c r="BM2">
+      <c r="BM2" s="4">
         <v>11.698</v>
       </c>
-      <c r="BN2">
+      <c r="BN2" s="4">
         <v>11.433999999999999</v>
       </c>
-      <c r="BO2">
+      <c r="BO2" s="4">
         <v>9.5350000000000001</v>
       </c>
-      <c r="BP2">
+      <c r="BP2" s="4">
         <v>11.138</v>
       </c>
-      <c r="BQ2">
+      <c r="BQ2" s="4">
         <v>11.375</v>
       </c>
-      <c r="BR2">
+      <c r="BR2" s="4">
         <v>9.2349999999999994</v>
       </c>
-      <c r="BS2">
+      <c r="BS2" s="4">
         <v>11.587999999999999</v>
       </c>
-      <c r="BT2">
+      <c r="BT2" s="4">
         <v>10.683</v>
       </c>
-      <c r="BU2">
+      <c r="BU2" s="4">
         <v>10.433</v>
       </c>
-      <c r="BV2">
+      <c r="BV2" s="4">
         <v>10.874000000000001</v>
       </c>
-      <c r="BW2">
+      <c r="BW2" s="4">
         <v>10.866</v>
       </c>
-      <c r="BX2">
+      <c r="BX2" s="4">
         <v>9.9659999999999993</v>
       </c>
-      <c r="BY2">
+      <c r="BY2" s="4">
         <v>10.738</v>
       </c>
-      <c r="BZ2">
+      <c r="BZ2" s="4">
         <v>11.015000000000001</v>
       </c>
-      <c r="CA2">
+      <c r="CA2" s="4">
         <v>10.965999999999999</v>
       </c>
-      <c r="CB2">
+      <c r="CB2" s="4">
         <v>10.371</v>
       </c>
-      <c r="CC2">
+      <c r="CC2" s="4">
         <v>10.756</v>
       </c>
-      <c r="CD2">
+      <c r="CD2" s="4">
         <v>10.414</v>
       </c>
-      <c r="CE2">
+      <c r="CE2" s="4">
         <v>10.723000000000001</v>
       </c>
-      <c r="CF2">
+      <c r="CF2" s="4">
         <v>12.534000000000001</v>
       </c>
-      <c r="CG2">
+      <c r="CG2" s="4">
         <v>12.385</v>
       </c>
-      <c r="CH2">
+      <c r="CH2" s="4">
         <v>10.645</v>
       </c>
-      <c r="CI2">
+      <c r="CI2" s="4">
         <v>11.420999999999999</v>
       </c>
-      <c r="CJ2">
+      <c r="CJ2" s="4">
         <v>10.244999999999999</v>
       </c>
-      <c r="CK2">
+      <c r="CK2" s="4">
         <v>10.662000000000001</v>
       </c>
-      <c r="CL2">
+      <c r="CL2" s="4">
         <v>9.8740000000000006</v>
       </c>
-      <c r="CM2">
+      <c r="CM2" s="4">
         <v>10.420999999999999</v>
       </c>
-      <c r="CN2">
+      <c r="CN2" s="4">
         <v>11.112</v>
       </c>
-      <c r="CO2">
+      <c r="CO2" s="4">
         <v>11.298999999999999</v>
       </c>
-      <c r="CP2">
+      <c r="CP2" s="4">
         <v>11.223000000000001</v>
       </c>
-      <c r="CQ2">
+      <c r="CQ2" s="4">
         <v>10.457000000000001</v>
       </c>
-      <c r="CR2">
+      <c r="CR2" s="4">
         <v>9.7059999999999995</v>
       </c>
-      <c r="CS2">
+      <c r="CS2" s="4">
         <v>11.563000000000001</v>
       </c>
-      <c r="CT2">
+      <c r="CT2" s="4">
         <v>12.71</v>
       </c>
-      <c r="CU2">
+      <c r="CU2" s="4">
         <v>10.401</v>
       </c>
-      <c r="CV2">
+      <c r="CV2" s="4">
         <v>10.436</v>
       </c>
-      <c r="CW2">
+      <c r="CW2" s="4">
         <v>11.11</v>
       </c>
-      <c r="CX2">
+      <c r="CX2" s="4">
         <v>11.818</v>
       </c>
     </row>
@@ -1552,9 +1560,9 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <f t="shared" si="0"/>
-        <v>18.285128571428569</v>
+        <v>18.310302631578953</v>
       </c>
       <c r="C3">
         <v>9.6579999999999995</v>
@@ -1857,312 +1865,312 @@
         <v>19.452999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:102" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
-        <f t="shared" si="0"/>
-        <v>7.8746142857142871</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="5">
+        <f>AVERAGE(C4:CX4)</f>
+        <v>7.8887300000000007</v>
+      </c>
+      <c r="C4" s="4">
         <v>7.7359999999999998</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>7.5640000000000001</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>8.4760000000000009</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="4">
         <v>7.2869999999999999</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <v>7.2869999999999999</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <v>7.9029999999999996</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="4">
         <v>7.6890000000000001</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="4">
         <v>7.5629999999999997</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="4">
         <v>7.7380000000000004</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="4">
         <v>8.7289999999999992</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="4">
         <v>8.3569999999999993</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="4">
         <v>7.2530000000000001</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="4">
         <v>8.0129999999999999</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="4">
         <v>7.4829999999999997</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="4">
         <v>7.58</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="4">
         <v>7.9349999999999996</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="4">
         <v>7.9210000000000003</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="4">
         <v>8.077</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="4">
         <v>7.6189999999999998</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="4">
         <v>7.4009999999999998</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="4">
         <v>7.774</v>
       </c>
-      <c r="X4">
+      <c r="X4" s="4">
         <v>7.7329999999999997</v>
       </c>
-      <c r="Y4">
+      <c r="Y4" s="4">
         <v>9.3480000000000008</v>
       </c>
-      <c r="Z4">
+      <c r="Z4" s="4">
         <v>7.7210000000000001</v>
       </c>
-      <c r="AA4">
+      <c r="AA4" s="4">
         <v>7.7290000000000001</v>
       </c>
-      <c r="AB4">
+      <c r="AB4" s="4">
         <v>7.9340000000000002</v>
       </c>
-      <c r="AC4">
+      <c r="AC4" s="4">
         <v>8.7309999999999999</v>
       </c>
-      <c r="AD4">
+      <c r="AD4" s="4">
         <v>7.6390000000000002</v>
       </c>
-      <c r="AE4">
+      <c r="AE4" s="4">
         <v>8.1809999999999992</v>
       </c>
-      <c r="AF4">
+      <c r="AF4" s="4">
         <v>7.8449999999999998</v>
       </c>
-      <c r="AG4">
+      <c r="AG4" s="4">
         <v>8.2569999999999997</v>
       </c>
-      <c r="AH4">
+      <c r="AH4" s="4">
         <v>8.0050000000000008</v>
       </c>
-      <c r="AI4">
+      <c r="AI4" s="4">
         <v>8.1850000000000005</v>
       </c>
-      <c r="AJ4">
+      <c r="AJ4" s="4">
         <v>8.0109999999999992</v>
       </c>
-      <c r="AK4">
+      <c r="AK4" s="4">
         <v>7.4459999999999997</v>
       </c>
-      <c r="AL4">
+      <c r="AL4" s="4">
         <v>7.891</v>
       </c>
-      <c r="AM4">
+      <c r="AM4" s="4">
         <v>7.8040000000000003</v>
       </c>
-      <c r="AN4">
+      <c r="AN4" s="4">
         <v>7.75</v>
       </c>
-      <c r="AO4">
+      <c r="AO4" s="4">
         <v>7.0949999999999998</v>
       </c>
-      <c r="AP4">
+      <c r="AP4" s="4">
         <v>7.1109999999999998</v>
       </c>
-      <c r="AQ4">
+      <c r="AQ4" s="4">
         <v>8.0440000000000005</v>
       </c>
-      <c r="AR4">
+      <c r="AR4" s="4">
         <v>7.7160000000000002</v>
       </c>
-      <c r="AS4">
+      <c r="AS4" s="4">
         <v>8.4920000000000009</v>
       </c>
-      <c r="AT4">
+      <c r="AT4" s="4">
         <v>7.835</v>
       </c>
-      <c r="AU4">
+      <c r="AU4" s="4">
         <v>8.2140000000000004</v>
       </c>
-      <c r="AV4">
+      <c r="AV4" s="4">
         <v>8.3789999999999996</v>
       </c>
-      <c r="AW4">
+      <c r="AW4" s="4">
         <v>8.6059999999999999</v>
       </c>
-      <c r="AX4">
+      <c r="AX4" s="4">
         <v>8.3040000000000003</v>
       </c>
-      <c r="AY4">
+      <c r="AY4" s="4">
         <v>7.2270000000000003</v>
       </c>
-      <c r="AZ4">
+      <c r="AZ4" s="4">
         <v>7.6840000000000002</v>
       </c>
-      <c r="BA4">
+      <c r="BA4" s="4">
         <v>7.7119999999999997</v>
       </c>
-      <c r="BB4">
+      <c r="BB4" s="4">
         <v>7.9180000000000001</v>
       </c>
-      <c r="BC4">
+      <c r="BC4" s="4">
         <v>7.5650000000000004</v>
       </c>
-      <c r="BD4">
+      <c r="BD4" s="4">
         <v>8.9030000000000005</v>
       </c>
-      <c r="BE4">
+      <c r="BE4" s="4">
         <v>8.3239999999999998</v>
       </c>
-      <c r="BF4">
+      <c r="BF4" s="4">
         <v>8.0920000000000005</v>
       </c>
-      <c r="BG4">
+      <c r="BG4" s="4">
         <v>8.0630000000000006</v>
       </c>
-      <c r="BH4">
+      <c r="BH4" s="4">
         <v>7.9630000000000001</v>
       </c>
-      <c r="BI4">
+      <c r="BI4" s="4">
         <v>7.6829999999999998</v>
       </c>
-      <c r="BJ4">
+      <c r="BJ4" s="4">
         <v>7.9980000000000002</v>
       </c>
-      <c r="BK4">
+      <c r="BK4" s="4">
         <v>7.883</v>
       </c>
-      <c r="BL4">
+      <c r="BL4" s="4">
         <v>8.548</v>
       </c>
-      <c r="BM4">
+      <c r="BM4" s="4">
         <v>7.5279999999999996</v>
       </c>
-      <c r="BN4">
+      <c r="BN4" s="4">
         <v>7.9370000000000003</v>
       </c>
-      <c r="BO4">
+      <c r="BO4" s="4">
         <v>6.9009999999999998</v>
       </c>
-      <c r="BP4">
+      <c r="BP4" s="4">
         <v>8.0459999999999994</v>
       </c>
-      <c r="BQ4">
+      <c r="BQ4" s="4">
         <v>7.3079999999999998</v>
       </c>
-      <c r="BR4">
+      <c r="BR4" s="4">
         <v>7.4589999999999996</v>
       </c>
-      <c r="BS4">
+      <c r="BS4" s="4">
         <v>8.0030000000000001</v>
       </c>
-      <c r="BT4">
+      <c r="BT4" s="4">
         <v>8.0299999999999994</v>
       </c>
-      <c r="BU4">
+      <c r="BU4" s="4">
         <v>8.1300000000000008</v>
       </c>
-      <c r="BV4">
+      <c r="BV4" s="4">
         <v>8.2940000000000005</v>
       </c>
-      <c r="BW4">
+      <c r="BW4" s="4">
         <v>7.8719999999999999</v>
       </c>
-      <c r="BX4">
+      <c r="BX4" s="4">
         <v>7.8319999999999999</v>
       </c>
-      <c r="BY4">
+      <c r="BY4" s="4">
         <v>7.9669999999999996</v>
       </c>
-      <c r="BZ4">
+      <c r="BZ4" s="4">
         <v>7.7469999999999999</v>
       </c>
-      <c r="CA4">
+      <c r="CA4" s="4">
         <v>8.2420000000000009</v>
       </c>
-      <c r="CB4">
+      <c r="CB4" s="4">
         <v>8.2059999999999995</v>
       </c>
-      <c r="CC4">
+      <c r="CC4" s="4">
         <v>7.8460000000000001</v>
       </c>
-      <c r="CD4">
+      <c r="CD4" s="4">
         <v>8.673</v>
       </c>
-      <c r="CE4">
+      <c r="CE4" s="4">
         <v>8.593</v>
       </c>
-      <c r="CF4">
+      <c r="CF4" s="4">
         <v>8.1720000000000006</v>
       </c>
-      <c r="CG4">
+      <c r="CG4" s="4">
         <v>8.2149999999999999</v>
       </c>
-      <c r="CH4">
+      <c r="CH4" s="4">
         <v>7.577</v>
       </c>
-      <c r="CI4">
+      <c r="CI4" s="4">
         <v>7.6139999999999999</v>
       </c>
-      <c r="CJ4">
+      <c r="CJ4" s="4">
         <v>8.1809999999999992</v>
       </c>
-      <c r="CK4">
+      <c r="CK4" s="4">
         <v>7.5170000000000003</v>
       </c>
-      <c r="CL4">
+      <c r="CL4" s="4">
         <v>8.0809999999999995</v>
       </c>
-      <c r="CM4">
+      <c r="CM4" s="4">
         <v>7.4139999999999997</v>
       </c>
-      <c r="CN4">
+      <c r="CN4" s="4">
         <v>7.4210000000000003</v>
       </c>
-      <c r="CO4">
+      <c r="CO4" s="4">
         <v>8.2010000000000005</v>
       </c>
-      <c r="CP4">
+      <c r="CP4" s="4">
         <v>7.8940000000000001</v>
       </c>
-      <c r="CQ4">
+      <c r="CQ4" s="4">
         <v>7.234</v>
       </c>
-      <c r="CR4">
+      <c r="CR4" s="4">
         <v>7.2610000000000001</v>
       </c>
-      <c r="CS4">
+      <c r="CS4" s="4">
         <v>8.1809999999999992</v>
       </c>
-      <c r="CT4">
+      <c r="CT4" s="4">
         <v>8.3279999999999994</v>
       </c>
-      <c r="CU4">
+      <c r="CU4" s="4">
         <v>7.3949999999999996</v>
       </c>
-      <c r="CV4">
+      <c r="CV4" s="4">
         <v>7.2759999999999998</v>
       </c>
-      <c r="CW4">
+      <c r="CW4" s="4">
         <v>7.9340000000000002</v>
       </c>
-      <c r="CX4">
+      <c r="CX4" s="4">
         <v>7.4089999999999998</v>
       </c>
     </row>
@@ -2172,7 +2180,7 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" si="0"/>
-        <v>7.6136571428571411</v>
+        <v>7.6134736842105255</v>
       </c>
       <c r="C5">
         <v>7.375</v>
@@ -2479,9 +2487,9 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="3">
         <f t="shared" si="0"/>
-        <v>7.4027142857142865</v>
+        <v>7.4112236842105235</v>
       </c>
       <c r="C6">
         <v>5.694</v>
@@ -2788,9 +2796,9 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="3">
         <f t="shared" si="0"/>
-        <v>1.2938571428571433</v>
+        <v>1.2966710526315788</v>
       </c>
       <c r="C7">
         <v>1.323</v>
@@ -3099,7 +3107,7 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" si="0"/>
-        <v>1.2922571428571432</v>
+        <v>1.2924473684210529</v>
       </c>
       <c r="C8">
         <v>1.2929999999999999</v>
@@ -3402,312 +3410,312 @@
         <v>1.1639999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:102" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
-        <f t="shared" si="0"/>
-        <v>0.53207142857142864</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="5">
+        <f>TRIMMEAN(C9:CX9,0.25)</f>
+        <v>0.53286842105263166</v>
+      </c>
+      <c r="C9" s="4">
         <v>0.84399999999999997</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>0.505</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <v>0.51300000000000001</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="4">
         <v>0.90700000000000003</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="4">
         <v>0.90700000000000003</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="4">
         <v>1</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="4">
         <v>0.28899999999999998</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="4">
         <v>0.59199999999999997</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="4">
         <v>0.63</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="4">
         <v>0.39900000000000002</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="4">
         <v>0.57099999999999995</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="4">
         <v>0.38</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="4">
         <v>0.313</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="4">
         <v>0.58899999999999997</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="4">
         <v>0.38400000000000001</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="4">
         <v>0.48899999999999999</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="4">
         <v>0.433</v>
       </c>
-      <c r="T9">
+      <c r="T9" s="4">
         <v>0.14799999999999999</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="4">
         <v>0.499</v>
       </c>
-      <c r="V9">
+      <c r="V9" s="4">
         <v>0.59799999999999998</v>
       </c>
-      <c r="W9">
+      <c r="W9" s="4">
         <v>0.39400000000000002</v>
       </c>
-      <c r="X9">
+      <c r="X9" s="4">
         <v>0.85199999999999998</v>
       </c>
-      <c r="Y9">
+      <c r="Y9" s="4">
         <v>0.14799999999999999</v>
       </c>
-      <c r="Z9">
+      <c r="Z9" s="4">
         <v>0.31900000000000001</v>
       </c>
-      <c r="AA9">
+      <c r="AA9" s="4">
         <v>0.63100000000000001</v>
       </c>
-      <c r="AB9">
+      <c r="AB9" s="4">
         <v>0.42699999999999999</v>
       </c>
-      <c r="AC9">
+      <c r="AC9" s="4">
         <v>0.72399999999999998</v>
       </c>
-      <c r="AD9">
+      <c r="AD9" s="4">
         <v>0.65400000000000003</v>
       </c>
-      <c r="AE9">
+      <c r="AE9" s="4">
         <v>0.77100000000000002</v>
       </c>
-      <c r="AF9">
+      <c r="AF9" s="4">
         <v>0.14799999999999999</v>
       </c>
-      <c r="AG9">
+      <c r="AG9" s="4">
         <v>0.28799999999999998</v>
       </c>
-      <c r="AH9">
+      <c r="AH9" s="4">
         <v>0.26700000000000002</v>
       </c>
-      <c r="AI9">
+      <c r="AI9" s="4">
         <v>0.48299999999999998</v>
       </c>
-      <c r="AJ9">
+      <c r="AJ9" s="4">
         <v>0.39300000000000002</v>
       </c>
-      <c r="AK9">
+      <c r="AK9" s="4">
         <v>0.14899999999999999</v>
       </c>
-      <c r="AL9">
+      <c r="AL9" s="4">
         <v>0.26</v>
       </c>
-      <c r="AM9">
+      <c r="AM9" s="4">
         <v>0.14899999999999999</v>
       </c>
-      <c r="AN9">
+      <c r="AN9" s="4">
         <v>0.47499999999999998</v>
       </c>
-      <c r="AO9">
+      <c r="AO9" s="4">
         <v>0.75700000000000001</v>
       </c>
-      <c r="AP9">
+      <c r="AP9" s="4">
         <v>0.71299999999999997</v>
       </c>
-      <c r="AQ9">
+      <c r="AQ9" s="4">
         <v>0.84899999999999998</v>
       </c>
-      <c r="AR9">
+      <c r="AR9" s="4">
         <v>0.64400000000000002</v>
       </c>
-      <c r="AS9">
+      <c r="AS9" s="4">
         <v>0.14799999999999999</v>
       </c>
-      <c r="AT9">
+      <c r="AT9" s="4">
         <v>0.70299999999999996</v>
       </c>
-      <c r="AU9">
+      <c r="AU9" s="4">
         <v>0.79200000000000004</v>
       </c>
-      <c r="AV9">
+      <c r="AV9" s="4">
         <v>0.28799999999999998</v>
       </c>
-      <c r="AW9">
+      <c r="AW9" s="4">
         <v>0.14799999999999999</v>
       </c>
-      <c r="AX9">
+      <c r="AX9" s="4">
         <v>0.72</v>
       </c>
-      <c r="AY9">
+      <c r="AY9" s="4">
         <v>0.53600000000000003</v>
       </c>
-      <c r="AZ9">
+      <c r="AZ9" s="4">
         <v>0.81899999999999995</v>
       </c>
-      <c r="BA9">
+      <c r="BA9" s="4">
         <v>1.0409999999999999</v>
       </c>
-      <c r="BB9">
+      <c r="BB9" s="4">
         <v>0.56200000000000006</v>
       </c>
-      <c r="BC9">
+      <c r="BC9" s="4">
         <v>0.65500000000000003</v>
       </c>
-      <c r="BD9">
+      <c r="BD9" s="4">
         <v>0.93</v>
       </c>
-      <c r="BE9">
+      <c r="BE9" s="4">
         <v>0.26400000000000001</v>
       </c>
-      <c r="BF9">
+      <c r="BF9" s="4">
         <v>0.29899999999999999</v>
       </c>
-      <c r="BG9">
+      <c r="BG9" s="4">
         <v>0.63700000000000001</v>
       </c>
-      <c r="BH9">
+      <c r="BH9" s="4">
         <v>0.35899999999999999</v>
       </c>
-      <c r="BI9">
+      <c r="BI9" s="4">
         <v>0.58899999999999997</v>
       </c>
-      <c r="BJ9">
+      <c r="BJ9" s="4">
         <v>1.4259999999999999</v>
       </c>
-      <c r="BK9">
+      <c r="BK9" s="4">
         <v>0.53100000000000003</v>
       </c>
-      <c r="BL9">
+      <c r="BL9" s="4">
         <v>0.67</v>
       </c>
-      <c r="BM9">
+      <c r="BM9" s="4">
         <v>0.14899999999999999</v>
       </c>
-      <c r="BN9">
+      <c r="BN9" s="4">
         <v>0.621</v>
       </c>
-      <c r="BO9">
+      <c r="BO9" s="4">
         <v>0.71899999999999997</v>
       </c>
-      <c r="BP9">
+      <c r="BP9" s="4">
         <v>0.74399999999999999</v>
       </c>
-      <c r="BQ9">
+      <c r="BQ9" s="4">
         <v>1.202</v>
       </c>
-      <c r="BR9">
+      <c r="BR9" s="4">
         <v>0.40600000000000003</v>
       </c>
-      <c r="BS9">
+      <c r="BS9" s="4">
         <v>0.16900000000000001</v>
       </c>
-      <c r="BT9">
+      <c r="BT9" s="4">
         <v>0.497</v>
       </c>
-      <c r="BU9">
+      <c r="BU9" s="4">
         <v>0.375</v>
       </c>
-      <c r="BV9">
+      <c r="BV9" s="4">
         <v>0.47099999999999997</v>
       </c>
-      <c r="BW9">
+      <c r="BW9" s="4">
         <v>0.82</v>
       </c>
-      <c r="BX9">
+      <c r="BX9" s="4">
         <v>0.57299999999999995</v>
       </c>
-      <c r="BY9">
+      <c r="BY9" s="4">
         <v>0.6</v>
       </c>
-      <c r="BZ9">
+      <c r="BZ9" s="4">
         <v>0.48699999999999999</v>
       </c>
-      <c r="CA9">
+      <c r="CA9" s="4">
         <v>0.46300000000000002</v>
       </c>
-      <c r="CB9">
+      <c r="CB9" s="4">
         <v>1.022</v>
       </c>
-      <c r="CC9">
+      <c r="CC9" s="4">
         <v>0.77300000000000002</v>
       </c>
-      <c r="CD9">
+      <c r="CD9" s="4">
         <v>0.14799999999999999</v>
       </c>
-      <c r="CE9">
+      <c r="CE9" s="4">
         <v>0.82299999999999995</v>
       </c>
-      <c r="CF9">
+      <c r="CF9" s="4">
         <v>0.15</v>
       </c>
-      <c r="CG9">
+      <c r="CG9" s="4">
         <v>0.379</v>
       </c>
-      <c r="CH9">
+      <c r="CH9" s="4">
         <v>0.41499999999999998</v>
       </c>
-      <c r="CI9">
+      <c r="CI9" s="4">
         <v>0.28499999999999998</v>
       </c>
-      <c r="CJ9">
+      <c r="CJ9" s="4">
         <v>0.434</v>
       </c>
-      <c r="CK9">
+      <c r="CK9" s="4">
         <v>0.14799999999999999</v>
       </c>
-      <c r="CL9">
+      <c r="CL9" s="4">
         <v>0.51500000000000001</v>
       </c>
-      <c r="CM9">
+      <c r="CM9" s="4">
         <v>0.628</v>
       </c>
-      <c r="CN9">
+      <c r="CN9" s="4">
         <v>0.45900000000000002</v>
       </c>
-      <c r="CO9">
+      <c r="CO9" s="4">
         <v>0.80100000000000005</v>
       </c>
-      <c r="CP9">
+      <c r="CP9" s="4">
         <v>0.57599999999999996</v>
       </c>
-      <c r="CQ9">
+      <c r="CQ9" s="4">
         <v>0.53700000000000003</v>
       </c>
-      <c r="CR9">
+      <c r="CR9" s="4">
         <v>0.96</v>
       </c>
-      <c r="CS9">
+      <c r="CS9" s="4">
         <v>0.29799999999999999</v>
       </c>
-      <c r="CT9">
+      <c r="CT9" s="4">
         <v>0.65700000000000003</v>
       </c>
-      <c r="CU9">
+      <c r="CU9" s="4">
         <v>0.58299999999999996</v>
       </c>
-      <c r="CV9">
+      <c r="CV9" s="4">
         <v>0.64800000000000002</v>
       </c>
-      <c r="CW9">
+      <c r="CW9" s="4">
         <v>0.40899999999999997</v>
       </c>
-      <c r="CX9">
+      <c r="CX9" s="4">
         <v>0.69399999999999995</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Perf - add final data from report analyzer
</commit_message>
<xml_diff>
--- a/docs/ReportAnalyzer-analyzers-versions/2017-04-21-systamio/aggregated.xlsx
+++ b/docs/ReportAnalyzer-analyzers-versions/2017-04-21-systamio/aggregated.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12525" windowHeight="2055"/>
   </bookViews>
   <sheets>
     <sheet name="aggregated" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,6 +391,18 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -552,9 +564,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - zvýraznenie1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -912,631 +928,631 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CX9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="115.28515625" customWidth="1"/>
+    <col min="1" max="1" width="113.7109375" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:102" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <f>TRIMMEAN(C1:CX1,0.3)</f>
-        <v>18.677542857142857</v>
-      </c>
-      <c r="C1">
+      <c r="B1" s="5">
+        <f t="shared" ref="B1:B8" si="0">TRIMMEAN(C1:CX1,0.25)</f>
+        <v>18.677302631578947</v>
+      </c>
+      <c r="C1" s="4">
         <v>17.544</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="4">
         <v>16.588999999999999</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="4">
         <v>19.074000000000002</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="4">
         <v>17.344000000000001</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="4">
         <v>17.344000000000001</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="4">
         <v>19.613</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="4">
         <v>17.036000000000001</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="4">
         <v>17.690999999999999</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="4">
         <v>18.082000000000001</v>
       </c>
-      <c r="L1">
+      <c r="L1" s="4">
         <v>19.175999999999998</v>
       </c>
-      <c r="M1">
+      <c r="M1" s="4">
         <v>18.564</v>
       </c>
-      <c r="N1">
+      <c r="N1" s="4">
         <v>18.408000000000001</v>
       </c>
-      <c r="O1">
+      <c r="O1" s="4">
         <v>18.68</v>
       </c>
-      <c r="P1">
+      <c r="P1" s="4">
         <v>20.388000000000002</v>
       </c>
-      <c r="Q1">
+      <c r="Q1" s="4">
         <v>18.803999999999998</v>
       </c>
-      <c r="R1">
+      <c r="R1" s="4">
         <v>19.309000000000001</v>
       </c>
-      <c r="S1">
+      <c r="S1" s="4">
         <v>18.527999999999999</v>
       </c>
-      <c r="T1">
+      <c r="T1" s="4">
         <v>18.872</v>
       </c>
-      <c r="U1">
+      <c r="U1" s="4">
         <v>17.89</v>
       </c>
-      <c r="V1">
+      <c r="V1" s="4">
         <v>17.59</v>
       </c>
-      <c r="W1">
+      <c r="W1" s="4">
         <v>18.664000000000001</v>
       </c>
-      <c r="X1">
+      <c r="X1" s="4">
         <v>19.373999999999999</v>
       </c>
-      <c r="Y1">
+      <c r="Y1" s="4">
         <v>18.707999999999998</v>
       </c>
-      <c r="Z1">
+      <c r="Z1" s="4">
         <v>17.459</v>
       </c>
-      <c r="AA1">
+      <c r="AA1" s="4">
         <v>17.803999999999998</v>
       </c>
-      <c r="AB1">
+      <c r="AB1" s="4">
         <v>17.677</v>
       </c>
-      <c r="AC1">
+      <c r="AC1" s="4">
         <v>18.739999999999998</v>
       </c>
-      <c r="AD1">
+      <c r="AD1" s="4">
         <v>18.986999999999998</v>
       </c>
-      <c r="AE1">
+      <c r="AE1" s="4">
         <v>18.242000000000001</v>
       </c>
-      <c r="AF1">
+      <c r="AF1" s="4">
         <v>19.564</v>
       </c>
-      <c r="AG1">
+      <c r="AG1" s="4">
         <v>18.87</v>
       </c>
-      <c r="AH1">
+      <c r="AH1" s="4">
         <v>20.196000000000002</v>
       </c>
-      <c r="AI1">
+      <c r="AI1" s="4">
         <v>20.678999999999998</v>
       </c>
-      <c r="AJ1">
+      <c r="AJ1" s="4">
         <v>17.565999999999999</v>
       </c>
-      <c r="AK1">
+      <c r="AK1" s="4">
         <v>18.518000000000001</v>
       </c>
-      <c r="AL1">
+      <c r="AL1" s="4">
         <v>18.027999999999999</v>
       </c>
-      <c r="AM1">
+      <c r="AM1" s="4">
         <v>20.768999999999998</v>
       </c>
-      <c r="AN1">
+      <c r="AN1" s="4">
         <v>17.443000000000001</v>
       </c>
-      <c r="AO1">
+      <c r="AO1" s="4">
         <v>19.082999999999998</v>
       </c>
-      <c r="AP1">
+      <c r="AP1" s="4">
         <v>19.202999999999999</v>
       </c>
-      <c r="AQ1">
+      <c r="AQ1" s="4">
         <v>20.273</v>
       </c>
-      <c r="AR1">
+      <c r="AR1" s="4">
         <v>19.864999999999998</v>
       </c>
-      <c r="AS1">
+      <c r="AS1" s="4">
         <v>19.643999999999998</v>
       </c>
-      <c r="AT1">
+      <c r="AT1" s="4">
         <v>18.931999999999999</v>
       </c>
-      <c r="AU1">
+      <c r="AU1" s="4">
         <v>19.420999999999999</v>
       </c>
-      <c r="AV1">
+      <c r="AV1" s="4">
         <v>19.773</v>
       </c>
-      <c r="AW1">
+      <c r="AW1" s="4">
         <v>17.692</v>
       </c>
-      <c r="AX1">
+      <c r="AX1" s="4">
         <v>19.192</v>
       </c>
-      <c r="AY1">
+      <c r="AY1" s="4">
         <v>17.617999999999999</v>
       </c>
-      <c r="AZ1">
+      <c r="AZ1" s="4">
         <v>18.521999999999998</v>
       </c>
-      <c r="BA1">
+      <c r="BA1" s="4">
         <v>19.625</v>
       </c>
-      <c r="BB1">
+      <c r="BB1" s="4">
         <v>20.379000000000001</v>
       </c>
-      <c r="BC1">
+      <c r="BC1" s="4">
         <v>18.344000000000001</v>
       </c>
-      <c r="BD1">
+      <c r="BD1" s="4">
         <v>18.774999999999999</v>
       </c>
-      <c r="BE1">
+      <c r="BE1" s="4">
         <v>18.443999999999999</v>
       </c>
-      <c r="BF1">
+      <c r="BF1" s="4">
         <v>18.189</v>
       </c>
-      <c r="BG1">
+      <c r="BG1" s="4">
         <v>19.292999999999999</v>
       </c>
-      <c r="BH1">
+      <c r="BH1" s="4">
         <v>18.693999999999999</v>
       </c>
-      <c r="BI1">
+      <c r="BI1" s="4">
         <v>16.683</v>
       </c>
-      <c r="BJ1">
+      <c r="BJ1" s="4">
         <v>17.803999999999998</v>
       </c>
-      <c r="BK1">
+      <c r="BK1" s="4">
         <v>18.149999999999999</v>
       </c>
-      <c r="BL1">
+      <c r="BL1" s="4">
         <v>17.655999999999999</v>
       </c>
-      <c r="BM1">
+      <c r="BM1" s="4">
         <v>18.696000000000002</v>
       </c>
-      <c r="BN1">
+      <c r="BN1" s="4">
         <v>18.021999999999998</v>
       </c>
-      <c r="BO1">
+      <c r="BO1" s="4">
         <v>17.765000000000001</v>
       </c>
-      <c r="BP1">
+      <c r="BP1" s="4">
         <v>20.225999999999999</v>
       </c>
-      <c r="BQ1">
+      <c r="BQ1" s="4">
         <v>17.597999999999999</v>
       </c>
-      <c r="BR1">
+      <c r="BR1" s="4">
         <v>18.123999999999999</v>
       </c>
-      <c r="BS1">
+      <c r="BS1" s="4">
         <v>18.809999999999999</v>
       </c>
-      <c r="BT1">
+      <c r="BT1" s="4">
         <v>20.317</v>
       </c>
-      <c r="BU1">
+      <c r="BU1" s="4">
         <v>19.983000000000001</v>
       </c>
-      <c r="BV1">
+      <c r="BV1" s="4">
         <v>17.507000000000001</v>
       </c>
-      <c r="BW1">
+      <c r="BW1" s="4">
         <v>19.207000000000001</v>
       </c>
-      <c r="BX1">
+      <c r="BX1" s="4">
         <v>18.11</v>
       </c>
-      <c r="BY1">
+      <c r="BY1" s="4">
         <v>17.661000000000001</v>
       </c>
-      <c r="BZ1">
+      <c r="BZ1" s="4">
         <v>19.515000000000001</v>
       </c>
-      <c r="CA1">
+      <c r="CA1" s="4">
         <v>18.959</v>
       </c>
-      <c r="CB1">
+      <c r="CB1" s="4">
         <v>19.169</v>
       </c>
-      <c r="CC1">
+      <c r="CC1" s="4">
         <v>18.556999999999999</v>
       </c>
-      <c r="CD1">
+      <c r="CD1" s="4">
         <v>18.905000000000001</v>
       </c>
-      <c r="CE1">
+      <c r="CE1" s="4">
         <v>17.917000000000002</v>
       </c>
-      <c r="CF1">
+      <c r="CF1" s="4">
         <v>19.536999999999999</v>
       </c>
-      <c r="CG1">
+      <c r="CG1" s="4">
         <v>19.853000000000002</v>
       </c>
-      <c r="CH1">
+      <c r="CH1" s="4">
         <v>18.591000000000001</v>
       </c>
-      <c r="CI1">
+      <c r="CI1" s="4">
         <v>19.742000000000001</v>
       </c>
-      <c r="CJ1">
+      <c r="CJ1" s="4">
         <v>17.789000000000001</v>
       </c>
-      <c r="CK1">
+      <c r="CK1" s="4">
         <v>19.053999999999998</v>
       </c>
-      <c r="CL1">
+      <c r="CL1" s="4">
         <v>18.030999999999999</v>
       </c>
-      <c r="CM1">
+      <c r="CM1" s="4">
         <v>17.901</v>
       </c>
-      <c r="CN1">
+      <c r="CN1" s="4">
         <v>19.079999999999998</v>
       </c>
-      <c r="CO1">
+      <c r="CO1" s="4">
         <v>19.943999999999999</v>
       </c>
-      <c r="CP1">
+      <c r="CP1" s="4">
         <v>19.454000000000001</v>
       </c>
-      <c r="CQ1">
+      <c r="CQ1" s="4">
         <v>19.449000000000002</v>
       </c>
-      <c r="CR1">
+      <c r="CR1" s="4">
         <v>18.654</v>
       </c>
-      <c r="CS1">
+      <c r="CS1" s="4">
         <v>19.66</v>
       </c>
-      <c r="CT1">
+      <c r="CT1" s="4">
         <v>18.609000000000002</v>
       </c>
-      <c r="CU1">
+      <c r="CU1" s="4">
         <v>17.481999999999999</v>
       </c>
-      <c r="CV1">
+      <c r="CV1" s="4">
         <v>19.074000000000002</v>
       </c>
-      <c r="CW1">
+      <c r="CW1" s="4">
         <v>19.545999999999999</v>
       </c>
-      <c r="CX1">
+      <c r="CX1" s="4">
         <v>18.367999999999999</v>
       </c>
     </row>
-    <row r="2" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:102" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <f t="shared" ref="B2:B9" si="0">TRIMMEAN(C2:CX2,0.3)</f>
-        <v>10.924828571428568</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="5">
+        <f t="shared" si="0"/>
+        <v>10.926947368421049</v>
+      </c>
+      <c r="C2" s="4">
         <v>10.371</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>10.845000000000001</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>11.015000000000001</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="4">
         <v>9.8460000000000001</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="4">
         <v>9.8460000000000001</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="4">
         <v>11.743</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="4">
         <v>10.239000000000001</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="4">
         <v>11.590999999999999</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="4">
         <v>12.148999999999999</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="4">
         <v>10.635999999999999</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="4">
         <v>10.585000000000001</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="4">
         <v>11.099</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="4">
         <v>10.472</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="4">
         <v>12.563000000000001</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="4">
         <v>11.840999999999999</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="4">
         <v>11.31</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="4">
         <v>9.6479999999999997</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="4">
         <v>11.042</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="4">
         <v>10.486000000000001</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="4">
         <v>10.138</v>
       </c>
-      <c r="W2">
+      <c r="W2" s="4">
         <v>10.464</v>
       </c>
-      <c r="X2">
+      <c r="X2" s="4">
         <v>11.715</v>
       </c>
-      <c r="Y2">
+      <c r="Y2" s="4">
         <v>10.621</v>
       </c>
-      <c r="Z2">
+      <c r="Z2" s="4">
         <v>10.685</v>
       </c>
-      <c r="AA2">
+      <c r="AA2" s="4">
         <v>9.5589999999999993</v>
       </c>
-      <c r="AB2">
+      <c r="AB2" s="4">
         <v>10.052</v>
       </c>
-      <c r="AC2">
+      <c r="AC2" s="4">
         <v>11.565</v>
       </c>
-      <c r="AD2">
+      <c r="AD2" s="4">
         <v>10.397</v>
       </c>
-      <c r="AE2">
+      <c r="AE2" s="4">
         <v>11.737</v>
       </c>
-      <c r="AF2">
+      <c r="AF2" s="4">
         <v>11.778</v>
       </c>
-      <c r="AG2">
+      <c r="AG2" s="4">
         <v>10.906000000000001</v>
       </c>
-      <c r="AH2">
+      <c r="AH2" s="4">
         <v>9.7449999999999992</v>
       </c>
-      <c r="AI2">
+      <c r="AI2" s="4">
         <v>10.098000000000001</v>
       </c>
-      <c r="AJ2">
+      <c r="AJ2" s="4">
         <v>11.778</v>
       </c>
-      <c r="AK2">
+      <c r="AK2" s="4">
         <v>10.927</v>
       </c>
-      <c r="AL2">
+      <c r="AL2" s="4">
         <v>12.253</v>
       </c>
-      <c r="AM2">
+      <c r="AM2" s="4">
         <v>11.244999999999999</v>
       </c>
-      <c r="AN2">
+      <c r="AN2" s="4">
         <v>10.602</v>
       </c>
-      <c r="AO2">
+      <c r="AO2" s="4">
         <v>10.071999999999999</v>
       </c>
-      <c r="AP2">
+      <c r="AP2" s="4">
         <v>12.243</v>
       </c>
-      <c r="AQ2">
+      <c r="AQ2" s="4">
         <v>10.680999999999999</v>
       </c>
-      <c r="AR2">
+      <c r="AR2" s="4">
         <v>11.067</v>
       </c>
-      <c r="AS2">
+      <c r="AS2" s="4">
         <v>11.965</v>
       </c>
-      <c r="AT2">
+      <c r="AT2" s="4">
         <v>11.894</v>
       </c>
-      <c r="AU2">
+      <c r="AU2" s="4">
         <v>11.247</v>
       </c>
-      <c r="AV2">
+      <c r="AV2" s="4">
         <v>10.958</v>
       </c>
-      <c r="AW2">
+      <c r="AW2" s="4">
         <v>11.316000000000001</v>
       </c>
-      <c r="AX2">
+      <c r="AX2" s="4">
         <v>10.727</v>
       </c>
-      <c r="AY2">
+      <c r="AY2" s="4">
         <v>10.71</v>
       </c>
-      <c r="AZ2">
+      <c r="AZ2" s="4">
         <v>11.805999999999999</v>
       </c>
-      <c r="BA2">
+      <c r="BA2" s="4">
         <v>10.545</v>
       </c>
-      <c r="BB2">
+      <c r="BB2" s="4">
         <v>11.407</v>
       </c>
-      <c r="BC2">
+      <c r="BC2" s="4">
         <v>11.67</v>
       </c>
-      <c r="BD2">
+      <c r="BD2" s="4">
         <v>10.87</v>
       </c>
-      <c r="BE2">
+      <c r="BE2" s="4">
         <v>12.151</v>
       </c>
-      <c r="BF2">
+      <c r="BF2" s="4">
         <v>11.102</v>
       </c>
-      <c r="BG2">
+      <c r="BG2" s="4">
         <v>10.391</v>
       </c>
-      <c r="BH2">
+      <c r="BH2" s="4">
         <v>10.324</v>
       </c>
-      <c r="BI2">
+      <c r="BI2" s="4">
         <v>10.89</v>
       </c>
-      <c r="BJ2">
+      <c r="BJ2" s="4">
         <v>12.163</v>
       </c>
-      <c r="BK2">
+      <c r="BK2" s="4">
         <v>9.9529999999999994</v>
       </c>
-      <c r="BL2">
+      <c r="BL2" s="4">
         <v>10.69</v>
       </c>
-      <c r="BM2">
+      <c r="BM2" s="4">
         <v>11.698</v>
       </c>
-      <c r="BN2">
+      <c r="BN2" s="4">
         <v>11.433999999999999</v>
       </c>
-      <c r="BO2">
+      <c r="BO2" s="4">
         <v>9.5350000000000001</v>
       </c>
-      <c r="BP2">
+      <c r="BP2" s="4">
         <v>11.138</v>
       </c>
-      <c r="BQ2">
+      <c r="BQ2" s="4">
         <v>11.375</v>
       </c>
-      <c r="BR2">
+      <c r="BR2" s="4">
         <v>9.2349999999999994</v>
       </c>
-      <c r="BS2">
+      <c r="BS2" s="4">
         <v>11.587999999999999</v>
       </c>
-      <c r="BT2">
+      <c r="BT2" s="4">
         <v>10.683</v>
       </c>
-      <c r="BU2">
+      <c r="BU2" s="4">
         <v>10.433</v>
       </c>
-      <c r="BV2">
+      <c r="BV2" s="4">
         <v>10.874000000000001</v>
       </c>
-      <c r="BW2">
+      <c r="BW2" s="4">
         <v>10.866</v>
       </c>
-      <c r="BX2">
+      <c r="BX2" s="4">
         <v>9.9659999999999993</v>
       </c>
-      <c r="BY2">
+      <c r="BY2" s="4">
         <v>10.738</v>
       </c>
-      <c r="BZ2">
+      <c r="BZ2" s="4">
         <v>11.015000000000001</v>
       </c>
-      <c r="CA2">
+      <c r="CA2" s="4">
         <v>10.965999999999999</v>
       </c>
-      <c r="CB2">
+      <c r="CB2" s="4">
         <v>10.371</v>
       </c>
-      <c r="CC2">
+      <c r="CC2" s="4">
         <v>10.756</v>
       </c>
-      <c r="CD2">
+      <c r="CD2" s="4">
         <v>10.414</v>
       </c>
-      <c r="CE2">
+      <c r="CE2" s="4">
         <v>10.723000000000001</v>
       </c>
-      <c r="CF2">
+      <c r="CF2" s="4">
         <v>12.534000000000001</v>
       </c>
-      <c r="CG2">
+      <c r="CG2" s="4">
         <v>12.385</v>
       </c>
-      <c r="CH2">
+      <c r="CH2" s="4">
         <v>10.645</v>
       </c>
-      <c r="CI2">
+      <c r="CI2" s="4">
         <v>11.420999999999999</v>
       </c>
-      <c r="CJ2">
+      <c r="CJ2" s="4">
         <v>10.244999999999999</v>
       </c>
-      <c r="CK2">
+      <c r="CK2" s="4">
         <v>10.662000000000001</v>
       </c>
-      <c r="CL2">
+      <c r="CL2" s="4">
         <v>9.8740000000000006</v>
       </c>
-      <c r="CM2">
+      <c r="CM2" s="4">
         <v>10.420999999999999</v>
       </c>
-      <c r="CN2">
+      <c r="CN2" s="4">
         <v>11.112</v>
       </c>
-      <c r="CO2">
+      <c r="CO2" s="4">
         <v>11.298999999999999</v>
       </c>
-      <c r="CP2">
+      <c r="CP2" s="4">
         <v>11.223000000000001</v>
       </c>
-      <c r="CQ2">
+      <c r="CQ2" s="4">
         <v>10.457000000000001</v>
       </c>
-      <c r="CR2">
+      <c r="CR2" s="4">
         <v>9.7059999999999995</v>
       </c>
-      <c r="CS2">
+      <c r="CS2" s="4">
         <v>11.563000000000001</v>
       </c>
-      <c r="CT2">
+      <c r="CT2" s="4">
         <v>12.71</v>
       </c>
-      <c r="CU2">
+      <c r="CU2" s="4">
         <v>10.401</v>
       </c>
-      <c r="CV2">
+      <c r="CV2" s="4">
         <v>10.436</v>
       </c>
-      <c r="CW2">
+      <c r="CW2" s="4">
         <v>11.11</v>
       </c>
-      <c r="CX2">
+      <c r="CX2" s="4">
         <v>11.818</v>
       </c>
     </row>
@@ -1544,9 +1560,9 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <f t="shared" si="0"/>
-        <v>18.285128571428569</v>
+        <v>18.310302631578953</v>
       </c>
       <c r="C3">
         <v>9.6579999999999995</v>
@@ -1849,322 +1865,322 @@
         <v>19.452999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:102" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <f t="shared" si="0"/>
-        <v>7.8746142857142871</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="5">
+        <f>AVERAGE(C4:CX4)</f>
+        <v>7.8887300000000007</v>
+      </c>
+      <c r="C4" s="4">
         <v>7.7359999999999998</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>7.5640000000000001</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>8.4760000000000009</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="4">
         <v>7.2869999999999999</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <v>7.2869999999999999</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <v>7.9029999999999996</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="4">
         <v>7.6890000000000001</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="4">
         <v>7.5629999999999997</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="4">
         <v>7.7380000000000004</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="4">
         <v>8.7289999999999992</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="4">
         <v>8.3569999999999993</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="4">
         <v>7.2530000000000001</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="4">
         <v>8.0129999999999999</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="4">
         <v>7.4829999999999997</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="4">
         <v>7.58</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="4">
         <v>7.9349999999999996</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="4">
         <v>7.9210000000000003</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="4">
         <v>8.077</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="4">
         <v>7.6189999999999998</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="4">
         <v>7.4009999999999998</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="4">
         <v>7.774</v>
       </c>
-      <c r="X4">
+      <c r="X4" s="4">
         <v>7.7329999999999997</v>
       </c>
-      <c r="Y4">
+      <c r="Y4" s="4">
         <v>9.3480000000000008</v>
       </c>
-      <c r="Z4">
+      <c r="Z4" s="4">
         <v>7.7210000000000001</v>
       </c>
-      <c r="AA4">
+      <c r="AA4" s="4">
         <v>7.7290000000000001</v>
       </c>
-      <c r="AB4">
+      <c r="AB4" s="4">
         <v>7.9340000000000002</v>
       </c>
-      <c r="AC4">
+      <c r="AC4" s="4">
         <v>8.7309999999999999</v>
       </c>
-      <c r="AD4">
+      <c r="AD4" s="4">
         <v>7.6390000000000002</v>
       </c>
-      <c r="AE4">
+      <c r="AE4" s="4">
         <v>8.1809999999999992</v>
       </c>
-      <c r="AF4">
+      <c r="AF4" s="4">
         <v>7.8449999999999998</v>
       </c>
-      <c r="AG4">
+      <c r="AG4" s="4">
         <v>8.2569999999999997</v>
       </c>
-      <c r="AH4">
+      <c r="AH4" s="4">
         <v>8.0050000000000008</v>
       </c>
-      <c r="AI4">
+      <c r="AI4" s="4">
         <v>8.1850000000000005</v>
       </c>
-      <c r="AJ4">
+      <c r="AJ4" s="4">
         <v>8.0109999999999992</v>
       </c>
-      <c r="AK4">
+      <c r="AK4" s="4">
         <v>7.4459999999999997</v>
       </c>
-      <c r="AL4">
+      <c r="AL4" s="4">
         <v>7.891</v>
       </c>
-      <c r="AM4">
+      <c r="AM4" s="4">
         <v>7.8040000000000003</v>
       </c>
-      <c r="AN4">
+      <c r="AN4" s="4">
         <v>7.75</v>
       </c>
-      <c r="AO4">
+      <c r="AO4" s="4">
         <v>7.0949999999999998</v>
       </c>
-      <c r="AP4">
+      <c r="AP4" s="4">
         <v>7.1109999999999998</v>
       </c>
-      <c r="AQ4">
+      <c r="AQ4" s="4">
         <v>8.0440000000000005</v>
       </c>
-      <c r="AR4">
+      <c r="AR4" s="4">
         <v>7.7160000000000002</v>
       </c>
-      <c r="AS4">
+      <c r="AS4" s="4">
         <v>8.4920000000000009</v>
       </c>
-      <c r="AT4">
+      <c r="AT4" s="4">
         <v>7.835</v>
       </c>
-      <c r="AU4">
+      <c r="AU4" s="4">
         <v>8.2140000000000004</v>
       </c>
-      <c r="AV4">
+      <c r="AV4" s="4">
         <v>8.3789999999999996</v>
       </c>
-      <c r="AW4">
+      <c r="AW4" s="4">
         <v>8.6059999999999999</v>
       </c>
-      <c r="AX4">
+      <c r="AX4" s="4">
         <v>8.3040000000000003</v>
       </c>
-      <c r="AY4">
+      <c r="AY4" s="4">
         <v>7.2270000000000003</v>
       </c>
-      <c r="AZ4">
+      <c r="AZ4" s="4">
         <v>7.6840000000000002</v>
       </c>
-      <c r="BA4">
+      <c r="BA4" s="4">
         <v>7.7119999999999997</v>
       </c>
-      <c r="BB4">
+      <c r="BB4" s="4">
         <v>7.9180000000000001</v>
       </c>
-      <c r="BC4">
+      <c r="BC4" s="4">
         <v>7.5650000000000004</v>
       </c>
-      <c r="BD4">
+      <c r="BD4" s="4">
         <v>8.9030000000000005</v>
       </c>
-      <c r="BE4">
+      <c r="BE4" s="4">
         <v>8.3239999999999998</v>
       </c>
-      <c r="BF4">
+      <c r="BF4" s="4">
         <v>8.0920000000000005</v>
       </c>
-      <c r="BG4">
+      <c r="BG4" s="4">
         <v>8.0630000000000006</v>
       </c>
-      <c r="BH4">
+      <c r="BH4" s="4">
         <v>7.9630000000000001</v>
       </c>
-      <c r="BI4">
+      <c r="BI4" s="4">
         <v>7.6829999999999998</v>
       </c>
-      <c r="BJ4">
+      <c r="BJ4" s="4">
         <v>7.9980000000000002</v>
       </c>
-      <c r="BK4">
+      <c r="BK4" s="4">
         <v>7.883</v>
       </c>
-      <c r="BL4">
+      <c r="BL4" s="4">
         <v>8.548</v>
       </c>
-      <c r="BM4">
+      <c r="BM4" s="4">
         <v>7.5279999999999996</v>
       </c>
-      <c r="BN4">
+      <c r="BN4" s="4">
         <v>7.9370000000000003</v>
       </c>
-      <c r="BO4">
+      <c r="BO4" s="4">
         <v>6.9009999999999998</v>
       </c>
-      <c r="BP4">
+      <c r="BP4" s="4">
         <v>8.0459999999999994</v>
       </c>
-      <c r="BQ4">
+      <c r="BQ4" s="4">
         <v>7.3079999999999998</v>
       </c>
-      <c r="BR4">
+      <c r="BR4" s="4">
         <v>7.4589999999999996</v>
       </c>
-      <c r="BS4">
+      <c r="BS4" s="4">
         <v>8.0030000000000001</v>
       </c>
-      <c r="BT4">
+      <c r="BT4" s="4">
         <v>8.0299999999999994</v>
       </c>
-      <c r="BU4">
+      <c r="BU4" s="4">
         <v>8.1300000000000008</v>
       </c>
-      <c r="BV4">
+      <c r="BV4" s="4">
         <v>8.2940000000000005</v>
       </c>
-      <c r="BW4">
+      <c r="BW4" s="4">
         <v>7.8719999999999999</v>
       </c>
-      <c r="BX4">
+      <c r="BX4" s="4">
         <v>7.8319999999999999</v>
       </c>
-      <c r="BY4">
+      <c r="BY4" s="4">
         <v>7.9669999999999996</v>
       </c>
-      <c r="BZ4">
+      <c r="BZ4" s="4">
         <v>7.7469999999999999</v>
       </c>
-      <c r="CA4">
+      <c r="CA4" s="4">
         <v>8.2420000000000009</v>
       </c>
-      <c r="CB4">
+      <c r="CB4" s="4">
         <v>8.2059999999999995</v>
       </c>
-      <c r="CC4">
+      <c r="CC4" s="4">
         <v>7.8460000000000001</v>
       </c>
-      <c r="CD4">
+      <c r="CD4" s="4">
         <v>8.673</v>
       </c>
-      <c r="CE4">
+      <c r="CE4" s="4">
         <v>8.593</v>
       </c>
-      <c r="CF4">
+      <c r="CF4" s="4">
         <v>8.1720000000000006</v>
       </c>
-      <c r="CG4">
+      <c r="CG4" s="4">
         <v>8.2149999999999999</v>
       </c>
-      <c r="CH4">
+      <c r="CH4" s="4">
         <v>7.577</v>
       </c>
-      <c r="CI4">
+      <c r="CI4" s="4">
         <v>7.6139999999999999</v>
       </c>
-      <c r="CJ4">
+      <c r="CJ4" s="4">
         <v>8.1809999999999992</v>
       </c>
-      <c r="CK4">
+      <c r="CK4" s="4">
         <v>7.5170000000000003</v>
       </c>
-      <c r="CL4">
+      <c r="CL4" s="4">
         <v>8.0809999999999995</v>
       </c>
-      <c r="CM4">
+      <c r="CM4" s="4">
         <v>7.4139999999999997</v>
       </c>
-      <c r="CN4">
+      <c r="CN4" s="4">
         <v>7.4210000000000003</v>
       </c>
-      <c r="CO4">
+      <c r="CO4" s="4">
         <v>8.2010000000000005</v>
       </c>
-      <c r="CP4">
+      <c r="CP4" s="4">
         <v>7.8940000000000001</v>
       </c>
-      <c r="CQ4">
+      <c r="CQ4" s="4">
         <v>7.234</v>
       </c>
-      <c r="CR4">
+      <c r="CR4" s="4">
         <v>7.2610000000000001</v>
       </c>
-      <c r="CS4">
+      <c r="CS4" s="4">
         <v>8.1809999999999992</v>
       </c>
-      <c r="CT4">
+      <c r="CT4" s="4">
         <v>8.3279999999999994</v>
       </c>
-      <c r="CU4">
+      <c r="CU4" s="4">
         <v>7.3949999999999996</v>
       </c>
-      <c r="CV4">
+      <c r="CV4" s="4">
         <v>7.2759999999999998</v>
       </c>
-      <c r="CW4">
+      <c r="CW4" s="4">
         <v>7.9340000000000002</v>
       </c>
-      <c r="CX4">
+      <c r="CX4" s="4">
         <v>7.4089999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="3">
         <f t="shared" si="0"/>
-        <v>7.6136571428571411</v>
+        <v>7.6134736842105255</v>
       </c>
       <c r="C5">
         <v>7.375</v>
@@ -2471,9 +2487,9 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="3">
         <f t="shared" si="0"/>
-        <v>7.4027142857142865</v>
+        <v>7.4112236842105235</v>
       </c>
       <c r="C6">
         <v>5.694</v>
@@ -2780,9 +2796,9 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="3">
         <f t="shared" si="0"/>
-        <v>1.2938571428571433</v>
+        <v>1.2966710526315788</v>
       </c>
       <c r="C7">
         <v>1.323</v>
@@ -3086,12 +3102,12 @@
       </c>
     </row>
     <row r="8" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="3">
         <f t="shared" si="0"/>
-        <v>1.2922571428571432</v>
+        <v>1.2924473684210529</v>
       </c>
       <c r="C8">
         <v>1.2929999999999999</v>
@@ -3394,312 +3410,312 @@
         <v>1.1639999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:102" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
-        <f t="shared" si="0"/>
-        <v>0.53207142857142864</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="5">
+        <f>TRIMMEAN(C9:CX9,0.25)</f>
+        <v>0.53286842105263166</v>
+      </c>
+      <c r="C9" s="4">
         <v>0.84399999999999997</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>0.505</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <v>0.51300000000000001</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="4">
         <v>0.90700000000000003</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="4">
         <v>0.90700000000000003</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="4">
         <v>1</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="4">
         <v>0.28899999999999998</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="4">
         <v>0.59199999999999997</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="4">
         <v>0.63</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="4">
         <v>0.39900000000000002</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="4">
         <v>0.57099999999999995</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="4">
         <v>0.38</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="4">
         <v>0.313</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="4">
         <v>0.58899999999999997</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="4">
         <v>0.38400000000000001</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="4">
         <v>0.48899999999999999</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="4">
         <v>0.433</v>
       </c>
-      <c r="T9">
+      <c r="T9" s="4">
         <v>0.14799999999999999</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="4">
         <v>0.499</v>
       </c>
-      <c r="V9">
+      <c r="V9" s="4">
         <v>0.59799999999999998</v>
       </c>
-      <c r="W9">
+      <c r="W9" s="4">
         <v>0.39400000000000002</v>
       </c>
-      <c r="X9">
+      <c r="X9" s="4">
         <v>0.85199999999999998</v>
       </c>
-      <c r="Y9">
+      <c r="Y9" s="4">
         <v>0.14799999999999999</v>
       </c>
-      <c r="Z9">
+      <c r="Z9" s="4">
         <v>0.31900000000000001</v>
       </c>
-      <c r="AA9">
+      <c r="AA9" s="4">
         <v>0.63100000000000001</v>
       </c>
-      <c r="AB9">
+      <c r="AB9" s="4">
         <v>0.42699999999999999</v>
       </c>
-      <c r="AC9">
+      <c r="AC9" s="4">
         <v>0.72399999999999998</v>
       </c>
-      <c r="AD9">
+      <c r="AD9" s="4">
         <v>0.65400000000000003</v>
       </c>
-      <c r="AE9">
+      <c r="AE9" s="4">
         <v>0.77100000000000002</v>
       </c>
-      <c r="AF9">
+      <c r="AF9" s="4">
         <v>0.14799999999999999</v>
       </c>
-      <c r="AG9">
+      <c r="AG9" s="4">
         <v>0.28799999999999998</v>
       </c>
-      <c r="AH9">
+      <c r="AH9" s="4">
         <v>0.26700000000000002</v>
       </c>
-      <c r="AI9">
+      <c r="AI9" s="4">
         <v>0.48299999999999998</v>
       </c>
-      <c r="AJ9">
+      <c r="AJ9" s="4">
         <v>0.39300000000000002</v>
       </c>
-      <c r="AK9">
+      <c r="AK9" s="4">
         <v>0.14899999999999999</v>
       </c>
-      <c r="AL9">
+      <c r="AL9" s="4">
         <v>0.26</v>
       </c>
-      <c r="AM9">
+      <c r="AM9" s="4">
         <v>0.14899999999999999</v>
       </c>
-      <c r="AN9">
+      <c r="AN9" s="4">
         <v>0.47499999999999998</v>
       </c>
-      <c r="AO9">
+      <c r="AO9" s="4">
         <v>0.75700000000000001</v>
       </c>
-      <c r="AP9">
+      <c r="AP9" s="4">
         <v>0.71299999999999997</v>
       </c>
-      <c r="AQ9">
+      <c r="AQ9" s="4">
         <v>0.84899999999999998</v>
       </c>
-      <c r="AR9">
+      <c r="AR9" s="4">
         <v>0.64400000000000002</v>
       </c>
-      <c r="AS9">
+      <c r="AS9" s="4">
         <v>0.14799999999999999</v>
       </c>
-      <c r="AT9">
+      <c r="AT9" s="4">
         <v>0.70299999999999996</v>
       </c>
-      <c r="AU9">
+      <c r="AU9" s="4">
         <v>0.79200000000000004</v>
       </c>
-      <c r="AV9">
+      <c r="AV9" s="4">
         <v>0.28799999999999998</v>
       </c>
-      <c r="AW9">
+      <c r="AW9" s="4">
         <v>0.14799999999999999</v>
       </c>
-      <c r="AX9">
+      <c r="AX9" s="4">
         <v>0.72</v>
       </c>
-      <c r="AY9">
+      <c r="AY9" s="4">
         <v>0.53600000000000003</v>
       </c>
-      <c r="AZ9">
+      <c r="AZ9" s="4">
         <v>0.81899999999999995</v>
       </c>
-      <c r="BA9">
+      <c r="BA9" s="4">
         <v>1.0409999999999999</v>
       </c>
-      <c r="BB9">
+      <c r="BB9" s="4">
         <v>0.56200000000000006</v>
       </c>
-      <c r="BC9">
+      <c r="BC9" s="4">
         <v>0.65500000000000003</v>
       </c>
-      <c r="BD9">
+      <c r="BD9" s="4">
         <v>0.93</v>
       </c>
-      <c r="BE9">
+      <c r="BE9" s="4">
         <v>0.26400000000000001</v>
       </c>
-      <c r="BF9">
+      <c r="BF9" s="4">
         <v>0.29899999999999999</v>
       </c>
-      <c r="BG9">
+      <c r="BG9" s="4">
         <v>0.63700000000000001</v>
       </c>
-      <c r="BH9">
+      <c r="BH9" s="4">
         <v>0.35899999999999999</v>
       </c>
-      <c r="BI9">
+      <c r="BI9" s="4">
         <v>0.58899999999999997</v>
       </c>
-      <c r="BJ9">
+      <c r="BJ9" s="4">
         <v>1.4259999999999999</v>
       </c>
-      <c r="BK9">
+      <c r="BK9" s="4">
         <v>0.53100000000000003</v>
       </c>
-      <c r="BL9">
+      <c r="BL9" s="4">
         <v>0.67</v>
       </c>
-      <c r="BM9">
+      <c r="BM9" s="4">
         <v>0.14899999999999999</v>
       </c>
-      <c r="BN9">
+      <c r="BN9" s="4">
         <v>0.621</v>
       </c>
-      <c r="BO9">
+      <c r="BO9" s="4">
         <v>0.71899999999999997</v>
       </c>
-      <c r="BP9">
+      <c r="BP9" s="4">
         <v>0.74399999999999999</v>
       </c>
-      <c r="BQ9">
+      <c r="BQ9" s="4">
         <v>1.202</v>
       </c>
-      <c r="BR9">
+      <c r="BR9" s="4">
         <v>0.40600000000000003</v>
       </c>
-      <c r="BS9">
+      <c r="BS9" s="4">
         <v>0.16900000000000001</v>
       </c>
-      <c r="BT9">
+      <c r="BT9" s="4">
         <v>0.497</v>
       </c>
-      <c r="BU9">
+      <c r="BU9" s="4">
         <v>0.375</v>
       </c>
-      <c r="BV9">
+      <c r="BV9" s="4">
         <v>0.47099999999999997</v>
       </c>
-      <c r="BW9">
+      <c r="BW9" s="4">
         <v>0.82</v>
       </c>
-      <c r="BX9">
+      <c r="BX9" s="4">
         <v>0.57299999999999995</v>
       </c>
-      <c r="BY9">
+      <c r="BY9" s="4">
         <v>0.6</v>
       </c>
-      <c r="BZ9">
+      <c r="BZ9" s="4">
         <v>0.48699999999999999</v>
       </c>
-      <c r="CA9">
+      <c r="CA9" s="4">
         <v>0.46300000000000002</v>
       </c>
-      <c r="CB9">
+      <c r="CB9" s="4">
         <v>1.022</v>
       </c>
-      <c r="CC9">
+      <c r="CC9" s="4">
         <v>0.77300000000000002</v>
       </c>
-      <c r="CD9">
+      <c r="CD9" s="4">
         <v>0.14799999999999999</v>
       </c>
-      <c r="CE9">
+      <c r="CE9" s="4">
         <v>0.82299999999999995</v>
       </c>
-      <c r="CF9">
+      <c r="CF9" s="4">
         <v>0.15</v>
       </c>
-      <c r="CG9">
+      <c r="CG9" s="4">
         <v>0.379</v>
       </c>
-      <c r="CH9">
+      <c r="CH9" s="4">
         <v>0.41499999999999998</v>
       </c>
-      <c r="CI9">
+      <c r="CI9" s="4">
         <v>0.28499999999999998</v>
       </c>
-      <c r="CJ9">
+      <c r="CJ9" s="4">
         <v>0.434</v>
       </c>
-      <c r="CK9">
+      <c r="CK9" s="4">
         <v>0.14799999999999999</v>
       </c>
-      <c r="CL9">
+      <c r="CL9" s="4">
         <v>0.51500000000000001</v>
       </c>
-      <c r="CM9">
+      <c r="CM9" s="4">
         <v>0.628</v>
       </c>
-      <c r="CN9">
+      <c r="CN9" s="4">
         <v>0.45900000000000002</v>
       </c>
-      <c r="CO9">
+      <c r="CO9" s="4">
         <v>0.80100000000000005</v>
       </c>
-      <c r="CP9">
+      <c r="CP9" s="4">
         <v>0.57599999999999996</v>
       </c>
-      <c r="CQ9">
+      <c r="CQ9" s="4">
         <v>0.53700000000000003</v>
       </c>
-      <c r="CR9">
+      <c r="CR9" s="4">
         <v>0.96</v>
       </c>
-      <c r="CS9">
+      <c r="CS9" s="4">
         <v>0.29799999999999999</v>
       </c>
-      <c r="CT9">
+      <c r="CT9" s="4">
         <v>0.65700000000000003</v>
       </c>
-      <c r="CU9">
+      <c r="CU9" s="4">
         <v>0.58299999999999996</v>
       </c>
-      <c r="CV9">
+      <c r="CV9" s="4">
         <v>0.64800000000000002</v>
       </c>
-      <c r="CW9">
+      <c r="CW9" s="4">
         <v>0.40899999999999997</v>
       </c>
-      <c r="CX9">
+      <c r="CX9" s="4">
         <v>0.69399999999999995</v>
       </c>
     </row>

</xml_diff>